<commit_message>
Update MONTO DE INTERVENCION.xlsx
</commit_message>
<xml_diff>
--- a/data/MONTO DE INTERVENCION.xlsx
+++ b/data/MONTO DE INTERVENCION.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Sentiment_and_news-Peru\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131793AB-3834-4F04-A38D-D51C6C2D2B22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6654B3-40C6-4E5F-9DD0-D84ADEC99A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{59004005-DD27-4AB7-BFE9-37738C3DC820}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>TCVENTA</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>tasa</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
@@ -438,14 +441,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A21FBE1D-30DE-41F9-BD07-26FF0FF320F1}">
   <dimension ref="A1:M220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="M24" sqref="M24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="11.42578125" style="5"/>
+    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" style="2" customWidth="1"/>
     <col min="9" max="10" width="11.42578125" style="2"/>
@@ -461,8 +465,11 @@
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="E1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F1" t="s">
         <v>0</v>

</xml_diff>